<commit_message>
quote model POC complete in stage
</commit_message>
<xml_diff>
--- a/ETL/SSIS/JDE Table Master.xlsx
+++ b/ETL/SSIS/JDE Table Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13956" uniqueCount="3758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13958" uniqueCount="3758">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -11057,24 +11057,15 @@
     <t>JDE Table Master - ETL Group</t>
   </si>
   <si>
-    <t>Updated 20 Mar 17</t>
-  </si>
-  <si>
     <t>CU</t>
   </si>
   <si>
     <t>User Defined Codes - ARCPCOM93</t>
   </si>
   <si>
-    <t>ETL Status?</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
-    <t>needed?</t>
-  </si>
-  <si>
     <t>IsItem</t>
   </si>
   <si>
@@ -11301,6 +11292,15 @@
   </si>
   <si>
     <t>NOCHARGE</t>
+  </si>
+  <si>
+    <t>ETL Status</t>
+  </si>
+  <si>
+    <t>Updated 30 Mar 17</t>
+  </si>
+  <si>
+    <t>zNO</t>
   </si>
 </sst>
 </file>
@@ -11470,7 +11470,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11653,12 +11653,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11868,7 +11862,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -11876,7 +11870,6 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -11957,7 +11950,55 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -12658,68 +12699,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:G12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:G12" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="A3:G12"/>
   <sortState ref="A2:G11">
     <sortCondition descending="1" ref="D1:D11"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="ATPRFR preference type"/>
-    <tableColumn id="7" name="Type Name" dataDxfId="31"/>
-    <tableColumn id="6" name="adjustment name" dataDxfId="30"/>
-    <tableColumn id="2" name="IsItem" dataDxfId="29"/>
-    <tableColumn id="3" name="IsBillto" dataDxfId="28"/>
-    <tableColumn id="4" name="ItemCust" dataDxfId="27"/>
-    <tableColumn id="5" name="CountOfADAST  adjustment name" dataDxfId="26"/>
+    <tableColumn id="7" name="Type Name" dataDxfId="37"/>
+    <tableColumn id="6" name="adjustment name" dataDxfId="36"/>
+    <tableColumn id="2" name="IsItem" dataDxfId="35"/>
+    <tableColumn id="3" name="IsBillto" dataDxfId="34"/>
+    <tableColumn id="4" name="ItemCust" dataDxfId="33"/>
+    <tableColumn id="5" name="CountOfADAST  adjustment name" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A15:D21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A15:D21" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A15:D21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="DRKY   user defined code" dataDxfId="20"/>
-    <tableColumn id="2" name="DRDL01 description" dataDxfId="19"/>
-    <tableColumn id="3" name="DRSY   product code" dataDxfId="18"/>
-    <tableColumn id="4" name="DRRT   user defined codes" dataDxfId="17"/>
+    <tableColumn id="1" name="DRKY   user defined code" dataDxfId="26"/>
+    <tableColumn id="2" name="DRDL01 description" dataDxfId="25"/>
+    <tableColumn id="3" name="DRSY   product code" dataDxfId="24"/>
+    <tableColumn id="4" name="DRRT   user defined codes" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A24:D35" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12" headerRowCellStyle="Normal_Pricing_1" dataCellStyle="Normal_Pricing_1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A24:D35" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18" headerRowCellStyle="Normal_Pricing_1" dataCellStyle="Normal_Pricing_1">
   <autoFilter ref="A24:D35"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="DRKY   user defined code" dataDxfId="11" dataCellStyle="Normal_Pricing_1"/>
-    <tableColumn id="2" name="DRDL01 description" dataDxfId="10" dataCellStyle="Normal_Pricing_1"/>
-    <tableColumn id="3" name="DRSY   product code" dataDxfId="9" dataCellStyle="Normal_Pricing_1"/>
-    <tableColumn id="4" name="DRRT   user defined codes" dataDxfId="8" dataCellStyle="Normal_Pricing_1"/>
+    <tableColumn id="1" name="DRKY   user defined code" dataDxfId="17" dataCellStyle="Normal_Pricing_1"/>
+    <tableColumn id="2" name="DRDL01 description" dataDxfId="16" dataCellStyle="Normal_Pricing_1"/>
+    <tableColumn id="3" name="DRSY   product code" dataDxfId="15" dataCellStyle="Normal_Pricing_1"/>
+    <tableColumn id="4" name="DRRT   user defined codes" dataDxfId="14" dataCellStyle="Normal_Pricing_1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F37" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A3:F37">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="AdvPrc"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F37" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A3:F37"/>
   <sortState ref="A4:F37">
-    <sortCondition ref="A3:A37"/>
+    <sortCondition sortBy="cellColor" ref="B3:B37" dxfId="1"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="TABLE_NAME"/>
-    <tableColumn id="6" name="ETL Status?"/>
-    <tableColumn id="2" name="Group" dataDxfId="5"/>
-    <tableColumn id="3" name="Priority" dataDxfId="4"/>
-    <tableColumn id="4" name="Pull" dataDxfId="3"/>
+    <tableColumn id="6" name="ETL Status"/>
+    <tableColumn id="2" name="Group" dataDxfId="11"/>
+    <tableColumn id="3" name="Priority" dataDxfId="10"/>
+    <tableColumn id="4" name="Pull" dataDxfId="9"/>
     <tableColumn id="5" name="TABLE_TEXT"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -12737,11 +12772,11 @@
     <tableColumn id="5" name="ROW_LENGTH"/>
     <tableColumn id="3" name="TABLE_TYPE"/>
     <tableColumn id="8" name="TABLE_SCHEMA"/>
-    <tableColumn id="9" name="LAST_ALTERED_TIMESTAMP" dataDxfId="2"/>
+    <tableColumn id="9" name="LAST_ALTERED_TIMESTAMP" dataDxfId="8"/>
     <tableColumn id="12" name="FILE_TYPE"/>
     <tableColumn id="28" name="TABLE_DEFINER"/>
-    <tableColumn id="32" name="Tag" dataDxfId="1"/>
-    <tableColumn id="7" name="T2" dataDxfId="0">
+    <tableColumn id="32" name="Tag" dataDxfId="7"/>
+    <tableColumn id="7" name="T2" dataDxfId="6">
       <calculatedColumnFormula>+VLOOKUP(Table1[[#This Row],[TABLE_NAME]],ETL!$A:$E,2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13017,7 +13052,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -13037,514 +13072,514 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>3750</v>
+      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3751</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" s="14" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>3705</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>3744</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3679</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>3680</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>3681</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>3686</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3699</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3692</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G4" s="8">
+        <v>25693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>3687</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3700</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>3693</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G5" s="8">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>3669</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3697</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3694</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="G6" s="8">
+        <v>326416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>3691</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3704</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3706</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="G7" s="8">
+        <v>163245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>3685</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3698</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G8" s="8">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>3688</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>3701</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G9" s="8">
+        <v>23642</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>3689</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>3702</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3752</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G10" s="8">
+        <v>186582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>3690</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3703</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>3753</v>
       </c>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="D11" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>3684</v>
+      </c>
+      <c r="G11" s="8">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>3682</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>3696</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>3754</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="D12" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>3683</v>
+      </c>
+      <c r="G12" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>3746</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B15" s="17" t="s">
+        <v>3747</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>3748</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>3749</v>
+      </c>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>3708</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="B16" s="10" t="s">
+        <v>3709</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>3710</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>3711</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>3713</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>3714</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>3716</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>3717</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>3718</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>3719</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>3747</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>3682</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>3683</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>3684</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="C24" s="18" t="s">
         <v>3748</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>3689</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>3702</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D24" s="18" t="s">
+        <v>3749</v>
+      </c>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>3721</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>3722</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>3695</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G4" s="9">
-        <v>25693</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>3690</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>3703</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>3696</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G5" s="9">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>3669</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>3700</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>3697</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="G6" s="9">
-        <v>326416</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>3694</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>3707</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>3709</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="G7" s="9">
-        <v>163245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>3688</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>3701</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G8" s="9">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>3704</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G9" s="9">
-        <v>23642</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>3692</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>3705</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>3755</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G10" s="9">
-        <v>186582</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>3693</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>3706</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>3756</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>3687</v>
-      </c>
-      <c r="G11" s="9">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>3685</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>3699</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>3757</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>3686</v>
-      </c>
-      <c r="G12" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>3749</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>3750</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>3751</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>3752</v>
-      </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>3711</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>3712</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>3713</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>3714</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>3715</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>3716</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>3717</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>3718</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>3719</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="D25" s="12" t="s">
         <v>3720</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>3721</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>3722</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>3710</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>3749</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>3750</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>3751</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>3752</v>
-      </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>3723</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>3724</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="C26" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>3725</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>3726</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="C27" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>3727</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>3728</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="C28" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>3729</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>3730</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="C29" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>3731</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>3732</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="C30" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>3733</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>3734</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="C31" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>3735</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>3736</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="C32" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>3737</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>3738</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="C33" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>3739</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>3740</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="C34" s="12" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>3741</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="B35" s="13" t="s">
         <v>3742</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>3743</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>3723</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>3744</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>3745</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>3723</v>
+      <c r="C35" s="13" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>3720</v>
       </c>
     </row>
   </sheetData>
@@ -13569,9 +13604,9 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13591,7 +13626,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>3676</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -13599,7 +13634,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3679</v>
+        <v>3755</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3659</v>
@@ -13614,254 +13649,280 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3649</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3644</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3678</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3667</v>
-      </c>
-      <c r="F4" t="s">
+        <v>3665</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3669</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>3678</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>3665</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3672</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3665</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3672</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>3651</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3660</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>3670</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>3664</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>3677</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>3676</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>492</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>3664</v>
-      </c>
-      <c r="F6" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>3663</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1149</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3663</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1150</v>
-      </c>
-    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>1668</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>4</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>3671</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>1669</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>3651</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="5" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="D10" s="7">
-        <v>3</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>3670</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>3652</v>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>1716</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1709</v>
+      <c r="A11" s="5" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3678</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="F11" t="s">
-        <v>1710</v>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>1732</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>1711</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>3680</v>
+      <c r="B12" s="5" t="s">
+        <v>3678</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>1712</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="5" t="s">
+        <v>3648</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="D13" s="7">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>1716</v>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>3653</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>3648</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="5" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>3665</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>3649</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>3667</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>3677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3650</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3757</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>3660</v>
       </c>
-      <c r="D14" s="7">
-        <v>2</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7" t="s">
-        <v>3653</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1723</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>3662</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3658</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>3662</v>
+      <c r="D16" s="5">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>1728</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>3660</v>
-      </c>
-      <c r="D17" s="7">
-        <v>5</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>1732</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>3665</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>3672</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>3644</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>3665</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>3669</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>3654</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>3663</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>3663</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3663</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>3534</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1880</v>
+        <v>1902</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>3663</v>
@@ -13870,12 +13931,12 @@
         <v>3534</v>
       </c>
       <c r="F20" t="s">
-        <v>1881</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1902</v>
+        <v>2414</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>3663</v>
@@ -13884,210 +13945,189 @@
         <v>3534</v>
       </c>
       <c r="F21" t="s">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2414</v>
+        <v>2473</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>3663</v>
+        <v>3666</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>3534</v>
       </c>
       <c r="F22" t="s">
-        <v>2415</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3645</v>
-      </c>
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>3667</v>
-      </c>
-      <c r="F23" t="s">
-        <v>3655</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>3660</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2422</v>
+        <v>2448</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>3663</v>
+        <v>3660</v>
       </c>
       <c r="F24" t="s">
-        <v>2423</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2424</v>
+        <v>2450</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>3663</v>
+        <v>3660</v>
       </c>
       <c r="F25" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2428</v>
+        <v>2644</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>3667</v>
+        <v>3668</v>
       </c>
       <c r="F26" t="s">
-        <v>2429</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2448</v>
+        <v>2721</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>3660</v>
+        <v>3661</v>
       </c>
       <c r="F27" t="s">
-        <v>2449</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2450</v>
+        <v>2725</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>3660</v>
+        <v>3661</v>
       </c>
       <c r="F28" t="s">
-        <v>2451</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3650</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>3681</v>
+        <v>2727</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>3660</v>
-      </c>
-      <c r="D29" s="5">
-        <v>6</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>12</v>
+        <v>3661</v>
       </c>
       <c r="F29" t="s">
-        <v>3656</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+        <v>2728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>3664</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>3662</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>3662</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>2455</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>3662</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F33" t="s">
         <v>2456</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>2473</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>3666</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>3534</v>
-      </c>
-      <c r="F31" t="s">
-        <v>2474</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>2618</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>3665</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7" t="s">
-        <v>3672</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>2619</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>2644</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>3668</v>
-      </c>
-      <c r="F33" t="s">
-        <v>2645</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>2667</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>3680</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>3665</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>2668</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>3663</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2721</v>
+        <v>2424</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>3661</v>
+        <v>3663</v>
       </c>
       <c r="F35" t="s">
-        <v>2722</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2725</v>
+        <v>3645</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>3661</v>
+        <v>3667</v>
       </c>
       <c r="F36" t="s">
-        <v>2726</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2727</v>
+        <v>2428</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>3661</v>
+        <v>3667</v>
       </c>
       <c r="F37" t="s">
-        <v>2728</v>
+        <v>2429</v>
       </c>
     </row>
   </sheetData>
@@ -14585,9 +14625,9 @@
       <c r="J14" t="s">
         <v>15</v>
       </c>
-      <c r="L14">
-        <f>+VLOOKUP(Table1[[#This Row],[TABLE_NAME]],ETL!$A:$E,2,0)</f>
-        <v>0</v>
+      <c r="L14" t="str">
+        <f>+VLOOKUP(Table1[[#This Row],[TABLE_NAME]],ETL!$A:$E,2,0)</f>
+        <v>DONE</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>